<commit_message>
Continued tweaking the gear ratio spreadsheet.
</commit_message>
<xml_diff>
--- a/notes/gear_ratios.xlsx
+++ b/notes/gear_ratios.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\spider_dropper\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F0812B-CF3E-4D2B-AE29-1F0814D595B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BF2591-2923-43B4-9D94-3F1B1FFCC22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16457" yWindow="0" windowWidth="16457" windowHeight="17914" xr2:uid="{E034330B-BFBD-48DE-B9DD-948610082F57}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ratios" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>ISO module</t>
   </si>
@@ -94,6 +95,9 @@
   </si>
   <si>
     <t>(to contain the index track)</t>
+  </si>
+  <si>
+    <t>Ratio of Diameters</t>
   </si>
 </sst>
 </file>
@@ -164,40 +168,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <strike/>
@@ -232,6 +224,1464 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Drive Teeth</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Ratios!$C$10:$C$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>73</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-73E4-47B5-AF60-68EC9399E8D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Winder Teeth</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Ratios!$G$10:$G$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-73E4-47B5-AF60-68EC9399E8D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Drive OD</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Ratios!$F$10:$F$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>91.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>94.5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>103.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>106.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>109.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>112.5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>112.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-73E4-47B5-AF60-68EC9399E8D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Spool OD</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Ratios!$M$10:$M$51</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>26.430975742619378</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.606738158033906</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.782500573448431</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.606738158033906</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28.606738158033906</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.309787819692012</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.606738158033906</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32.715887143008239</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36.055373035884273</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39.3948589287603</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42.734344821636327</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>46.073830714512354</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>49.413316607388396</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>52.752802500264416</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>56.092288393140457</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>59.431774286016477</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>62.771260178892504</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>66.110746071768546</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>69.450231964644559</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>72.7897178575206</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>76.129203750396627</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>79.468689643272654</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>82.808175536148681</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>86.147661429024708</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>89.48714732190075</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>92.826633214776791</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>94.247691041532534</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>95.609538125506802</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>96.915799614216809</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>98.169810643378426</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>101.24213766482437</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>102.38673008457876</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>103.48729971895794</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>104.54633842373795</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>107.44476014208318</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>108.41090071486492</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>109.34190890318186</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>110.23966679905892</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>112.98281592534995</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>113.80094812091045</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>114.75034566041005</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>117.35401262773713</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-73E4-47B5-AF60-68EC9399E8D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1233786047"/>
+        <c:axId val="1233786527"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1233786047"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1233786527"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1233786527"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1233786047"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>10886</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>5443</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>5443</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BD4B7CE-72DE-72F8-46A6-963F257FD8DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -531,10 +1981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C1AACE9-797C-4CC1-8EA8-81631CAC12B7}">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -551,9 +2001,10 @@
     <col min="11" max="11" width="11.4609375" customWidth="1"/>
     <col min="12" max="12" width="15.07421875" customWidth="1"/>
     <col min="13" max="13" width="14.53515625" customWidth="1"/>
+    <col min="14" max="14" width="14.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -564,7 +2015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -572,7 +2023,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -587,7 +2038,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -598,7 +2049,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -609,7 +2060,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -620,2249 +2071,2420 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="3" t="s">
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="5"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="9"/>
       <c r="J8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="7"/>
-      <c r="L8" s="3" t="s">
+      <c r="K8" s="4"/>
+      <c r="L8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="M8" s="5"/>
-    </row>
-    <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="6" t="s">
+      <c r="M8" s="9"/>
+      <c r="N8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="L9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M9" s="7" t="s">
+      <c r="M9" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10">
-        <f>A10*25.4</f>
+        <f t="shared" ref="B10:B51" si="0">A10*25.4</f>
         <v>25.4</v>
       </c>
       <c r="C10">
         <v>57</v>
       </c>
       <c r="D10">
-        <f>_xlfn.CEILING.MATH(0.8*C10)</f>
+        <f t="shared" ref="D10:D51" si="1">_xlfn.CEILING.MATH(0.8*C10)</f>
         <v>46</v>
       </c>
       <c r="E10">
-        <f>C10*$C$1</f>
+        <f t="shared" ref="E10:E51" si="2">C10*$C$1</f>
         <v>85.5</v>
       </c>
       <c r="F10">
-        <f>E10+2*$C$1</f>
+        <f t="shared" ref="F10:F51" si="3">E10+2*$C$1</f>
         <v>88.5</v>
       </c>
       <c r="G10">
         <v>139</v>
       </c>
       <c r="H10">
-        <f>G10*$C$1</f>
+        <f t="shared" ref="H10:H51" si="4">G10*$C$1</f>
         <v>208.5</v>
       </c>
       <c r="I10">
-        <f>H10+2*$C$1</f>
+        <f t="shared" ref="I10:I51" si="5">H10+2*$C$1</f>
         <v>211.5</v>
       </c>
       <c r="J10">
-        <f>(E10+H10)/2</f>
+        <f t="shared" ref="J10:J51" si="6">(E10+H10)/2</f>
         <v>147</v>
       </c>
-      <c r="K10" s="9">
-        <f>D10/G10</f>
+      <c r="K10" s="5">
+        <f t="shared" ref="K10:K51" si="7">D10/G10</f>
         <v>0.33093525179856115</v>
       </c>
-      <c r="L10" s="9">
-        <f>B10/K10/PI()</f>
+      <c r="L10" s="5">
+        <f t="shared" ref="L10:L51" si="8">B10/K10/PI()</f>
         <v>24.430975742619378</v>
       </c>
-      <c r="M10" s="9">
-        <f>L10 + 4*$C$6*_xlfn.CEILING.MATH(K10)</f>
+      <c r="M10" s="5">
+        <f t="shared" ref="M10:M51" si="9">L10 + 4*$C$6*_xlfn.CEILING.MATH(K10)</f>
         <v>26.430975742619378</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N10" s="10">
+        <f>F10/M10</f>
+        <v>3.3483440362474268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11">
-        <f>A11*25.4</f>
+        <f t="shared" si="0"/>
         <v>50.8</v>
       </c>
       <c r="C11">
         <v>57</v>
       </c>
       <c r="D11">
-        <f>_xlfn.CEILING.MATH(0.8*C11)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E11">
-        <f>C11*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F11">
-        <f>E11+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G11">
         <v>70</v>
       </c>
       <c r="H11">
-        <f>G11*$C$1</f>
+        <f t="shared" si="4"/>
         <v>105</v>
       </c>
       <c r="I11">
-        <f>H11+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>108</v>
       </c>
       <c r="J11">
-        <f>(E11+H11)/2</f>
+        <f t="shared" si="6"/>
         <v>95.25</v>
       </c>
-      <c r="K11" s="9">
-        <f>D11/G11</f>
+      <c r="K11" s="5">
+        <f t="shared" si="7"/>
         <v>0.65714285714285714</v>
       </c>
-      <c r="L11" s="9">
-        <f>B11/K11/PI()</f>
+      <c r="L11" s="5">
+        <f t="shared" si="8"/>
         <v>24.606738158033906</v>
       </c>
-      <c r="M11" s="9">
-        <f>L11 + 4*$C$6*_xlfn.CEILING.MATH(K11)</f>
+      <c r="M11" s="5">
+        <f t="shared" si="9"/>
         <v>26.606738158033906</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N11" s="10">
+        <f t="shared" ref="N11:N51" si="10">F11/M11</f>
+        <v>3.3262250890862179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>3</v>
       </c>
       <c r="B12">
-        <f>A12*25.4</f>
+        <f t="shared" si="0"/>
         <v>76.199999999999989</v>
       </c>
       <c r="C12">
         <v>57</v>
       </c>
       <c r="D12">
-        <f>_xlfn.CEILING.MATH(0.8*C12)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E12">
-        <f>C12*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F12">
-        <f>E12+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G12">
         <v>47</v>
       </c>
       <c r="H12">
-        <f>G12*$C$1</f>
+        <f t="shared" si="4"/>
         <v>70.5</v>
       </c>
       <c r="I12">
-        <f>H12+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>73.5</v>
       </c>
       <c r="J12">
-        <f>(E12+H12)/2</f>
+        <f t="shared" si="6"/>
         <v>78</v>
       </c>
-      <c r="K12" s="9">
-        <f>D12/G12</f>
+      <c r="K12" s="5">
+        <f t="shared" si="7"/>
         <v>0.97872340425531912</v>
       </c>
-      <c r="L12" s="9">
-        <f>B12/K12/PI()</f>
+      <c r="L12" s="5">
+        <f t="shared" si="8"/>
         <v>24.782500573448431</v>
       </c>
-      <c r="M12" s="9">
-        <f>L12 + 4*$C$6*_xlfn.CEILING.MATH(K12)</f>
+      <c r="M12" s="5">
+        <f t="shared" si="9"/>
         <v>26.782500573448431</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N12" s="10">
+        <f t="shared" si="10"/>
+        <v>3.3043964568318507</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>4</v>
       </c>
       <c r="B13">
-        <f>A13*25.4</f>
+        <f t="shared" si="0"/>
         <v>101.6</v>
       </c>
       <c r="C13">
         <v>57</v>
       </c>
       <c r="D13">
-        <f>_xlfn.CEILING.MATH(0.8*C13)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E13">
-        <f>C13*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F13">
-        <f>E13+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G13">
         <v>35</v>
       </c>
       <c r="H13">
-        <f>G13*$C$1</f>
+        <f t="shared" si="4"/>
         <v>52.5</v>
       </c>
       <c r="I13">
-        <f>H13+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>55.5</v>
       </c>
       <c r="J13">
-        <f>(E13+H13)/2</f>
+        <f t="shared" si="6"/>
         <v>69</v>
       </c>
-      <c r="K13" s="9">
-        <f>D13/G13</f>
+      <c r="K13" s="5">
+        <f t="shared" si="7"/>
         <v>1.3142857142857143</v>
       </c>
-      <c r="L13" s="9">
-        <f>B13/K13/PI()</f>
+      <c r="L13" s="5">
+        <f t="shared" si="8"/>
         <v>24.606738158033906</v>
       </c>
-      <c r="M13" s="9">
-        <f>L13 + 4*$C$6*_xlfn.CEILING.MATH(K13)</f>
+      <c r="M13" s="5">
+        <f t="shared" si="9"/>
         <v>28.606738158033906</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N13" s="10">
+        <f t="shared" si="10"/>
+        <v>3.0936767243820036</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>5</v>
       </c>
       <c r="B14">
-        <f>A14*25.4</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="C14">
         <v>57</v>
       </c>
       <c r="D14">
-        <f>_xlfn.CEILING.MATH(0.8*C14)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E14">
-        <f>C14*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F14">
-        <f>E14+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G14">
         <v>28</v>
       </c>
       <c r="H14">
-        <f>G14*$C$1</f>
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
       <c r="I14">
-        <f>H14+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="J14">
-        <f>(E14+H14)/2</f>
+        <f t="shared" si="6"/>
         <v>63.75</v>
       </c>
-      <c r="K14" s="9">
-        <f>D14/G14</f>
+      <c r="K14" s="5">
+        <f t="shared" si="7"/>
         <v>1.6428571428571428</v>
       </c>
-      <c r="L14" s="9">
-        <f>B14/K14/PI()</f>
+      <c r="L14" s="5">
+        <f t="shared" si="8"/>
         <v>24.606738158033906</v>
       </c>
-      <c r="M14" s="9">
-        <f>L14 + 4*$C$6*_xlfn.CEILING.MATH(K14)</f>
+      <c r="M14" s="5">
+        <f t="shared" si="9"/>
         <v>28.606738158033906</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N14" s="10">
+        <f t="shared" si="10"/>
+        <v>3.0936767243820036</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>6</v>
       </c>
       <c r="B15">
-        <f>A15*25.4</f>
+        <f t="shared" si="0"/>
         <v>152.39999999999998</v>
       </c>
       <c r="C15">
         <v>57</v>
       </c>
       <c r="D15">
-        <f>_xlfn.CEILING.MATH(0.8*C15)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E15">
-        <f>C15*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F15">
-        <f>E15+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G15">
         <v>24</v>
       </c>
       <c r="H15">
-        <f>G15*$C$1</f>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="I15">
-        <f>H15+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>39</v>
       </c>
       <c r="J15">
-        <f>(E15+H15)/2</f>
+        <f t="shared" si="6"/>
         <v>60.75</v>
       </c>
-      <c r="K15" s="9">
-        <f>D15/G15</f>
+      <c r="K15" s="5">
+        <f t="shared" si="7"/>
         <v>1.9166666666666667</v>
       </c>
-      <c r="L15" s="9">
-        <f>B15/K15/PI()</f>
+      <c r="L15" s="5">
+        <f t="shared" si="8"/>
         <v>25.309787819692012</v>
       </c>
-      <c r="M15" s="9">
-        <f>L15 + 4*$C$6*_xlfn.CEILING.MATH(K15)</f>
+      <c r="M15" s="5">
+        <f t="shared" si="9"/>
         <v>29.309787819692012</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N15" s="10">
+        <f t="shared" si="10"/>
+        <v>3.0194691460898455</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>7</v>
       </c>
       <c r="B16">
-        <f>A16*25.4</f>
+        <f t="shared" si="0"/>
         <v>177.79999999999998</v>
       </c>
       <c r="C16">
         <v>57</v>
       </c>
       <c r="D16">
-        <f>_xlfn.CEILING.MATH(0.8*C16)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E16">
-        <f>C16*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F16">
-        <f>E16+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G16">
         <v>20</v>
       </c>
       <c r="H16">
-        <f>G16*$C$1</f>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="I16">
-        <f>H16+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
       <c r="J16">
-        <f>(E16+H16)/2</f>
+        <f t="shared" si="6"/>
         <v>57.75</v>
       </c>
-      <c r="K16" s="9">
-        <f>D16/G16</f>
+      <c r="K16" s="5">
+        <f t="shared" si="7"/>
         <v>2.2999999999999998</v>
       </c>
-      <c r="L16" s="9">
-        <f>B16/K16/PI()</f>
+      <c r="L16" s="5">
+        <f t="shared" si="8"/>
         <v>24.606738158033906</v>
       </c>
-      <c r="M16" s="9">
-        <f>L16 + 4*$C$6*_xlfn.CEILING.MATH(K16)</f>
+      <c r="M16" s="5">
+        <f t="shared" si="9"/>
         <v>30.606738158033906</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N16" s="10">
+        <f t="shared" si="10"/>
+        <v>2.891520146414877</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>8</v>
       </c>
       <c r="B17">
-        <f>A17*25.4</f>
+        <f t="shared" si="0"/>
         <v>203.2</v>
       </c>
       <c r="C17">
         <v>57</v>
       </c>
       <c r="D17">
-        <f>_xlfn.CEILING.MATH(0.8*C17)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E17">
-        <f>C17*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F17">
-        <f>E17+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G17">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" ref="G17:G51" si="11">_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
         <v>19</v>
       </c>
       <c r="H17">
-        <f>G17*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I17">
-        <f>H17+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J17">
-        <f>(E17+H17)/2</f>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="K17" s="9">
-        <f>D17/G17</f>
+      <c r="K17" s="5">
+        <f t="shared" si="7"/>
         <v>2.4210526315789473</v>
       </c>
-      <c r="L17" s="9">
-        <f>B17/K17/PI()</f>
+      <c r="L17" s="5">
+        <f t="shared" si="8"/>
         <v>26.715887143008239</v>
       </c>
-      <c r="M17" s="9">
-        <f>L17 + 4*$C$6*_xlfn.CEILING.MATH(K17)</f>
+      <c r="M17" s="5">
+        <f t="shared" si="9"/>
         <v>32.715887143008239</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N17" s="10">
+        <f t="shared" si="10"/>
+        <v>2.7051077543197071</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>9</v>
       </c>
       <c r="B18">
-        <f>A18*25.4</f>
+        <f t="shared" si="0"/>
         <v>228.6</v>
       </c>
       <c r="C18">
         <v>57</v>
       </c>
       <c r="D18">
-        <f>_xlfn.CEILING.MATH(0.8*C18)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E18">
-        <f>C18*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F18">
-        <f>E18+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G18">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H18">
-        <f>G18*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I18">
-        <f>H18+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J18">
-        <f>(E18+H18)/2</f>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="K18" s="9">
-        <f>D18/G18</f>
+      <c r="K18" s="5">
+        <f t="shared" si="7"/>
         <v>2.4210526315789473</v>
       </c>
-      <c r="L18" s="9">
-        <f>B18/K18/PI()</f>
+      <c r="L18" s="5">
+        <f t="shared" si="8"/>
         <v>30.055373035884273</v>
       </c>
-      <c r="M18" s="9">
-        <f>L18 + 4*$C$6*_xlfn.CEILING.MATH(K18)</f>
+      <c r="M18" s="5">
+        <f t="shared" si="9"/>
         <v>36.055373035884273</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N18" s="10">
+        <f t="shared" si="10"/>
+        <v>2.4545578799564765</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>10</v>
       </c>
       <c r="B19">
-        <f>A19*25.4</f>
+        <f t="shared" si="0"/>
         <v>254</v>
       </c>
       <c r="C19">
         <v>57</v>
       </c>
       <c r="D19">
-        <f>_xlfn.CEILING.MATH(0.8*C19)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E19">
-        <f>C19*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F19">
-        <f>E19+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G19">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H19">
-        <f>G19*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I19">
-        <f>H19+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J19">
-        <f>(E19+H19)/2</f>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="K19" s="9">
-        <f>D19/G19</f>
+      <c r="K19" s="5">
+        <f t="shared" si="7"/>
         <v>2.4210526315789473</v>
       </c>
-      <c r="L19" s="9">
-        <f>B19/K19/PI()</f>
+      <c r="L19" s="5">
+        <f t="shared" si="8"/>
         <v>33.3948589287603</v>
       </c>
-      <c r="M19" s="9">
-        <f>L19 + 4*$C$6*_xlfn.CEILING.MATH(K19)</f>
+      <c r="M19" s="5">
+        <f t="shared" si="9"/>
         <v>39.3948589287603</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N19" s="10">
+        <f t="shared" si="10"/>
+        <v>2.2464860239768591</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>11</v>
       </c>
       <c r="B20">
-        <f>A20*25.4</f>
+        <f t="shared" si="0"/>
         <v>279.39999999999998</v>
       </c>
       <c r="C20">
         <v>57</v>
       </c>
       <c r="D20">
-        <f>_xlfn.CEILING.MATH(0.8*C20)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E20">
-        <f>C20*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F20">
-        <f>E20+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G20">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H20">
-        <f>G20*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I20">
-        <f>H20+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J20">
-        <f>(E20+H20)/2</f>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="K20" s="9">
-        <f>D20/G20</f>
+      <c r="K20" s="5">
+        <f t="shared" si="7"/>
         <v>2.4210526315789473</v>
       </c>
-      <c r="L20" s="9">
-        <f>B20/K20/PI()</f>
+      <c r="L20" s="5">
+        <f t="shared" si="8"/>
         <v>36.734344821636327</v>
       </c>
-      <c r="M20" s="9">
-        <f>L20 + 4*$C$6*_xlfn.CEILING.MATH(K20)</f>
+      <c r="M20" s="5">
+        <f t="shared" si="9"/>
         <v>42.734344821636327</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N20" s="10">
+        <f t="shared" si="10"/>
+        <v>2.070933820779969</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>12</v>
       </c>
       <c r="B21">
-        <f>A21*25.4</f>
+        <f t="shared" si="0"/>
         <v>304.79999999999995</v>
       </c>
       <c r="C21">
         <v>57</v>
       </c>
       <c r="D21">
-        <f>_xlfn.CEILING.MATH(0.8*C21)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E21">
-        <f>C21*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F21">
-        <f>E21+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G21">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H21">
-        <f>G21*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I21">
-        <f>H21+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J21">
-        <f>(E21+H21)/2</f>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="K21" s="9">
-        <f>D21/G21</f>
+      <c r="K21" s="5">
+        <f t="shared" si="7"/>
         <v>2.4210526315789473</v>
       </c>
-      <c r="L21" s="9">
-        <f>B21/K21/PI()</f>
+      <c r="L21" s="5">
+        <f t="shared" si="8"/>
         <v>40.073830714512354</v>
       </c>
-      <c r="M21" s="9">
-        <f>L21 + 4*$C$6*_xlfn.CEILING.MATH(K21)</f>
+      <c r="M21" s="5">
+        <f t="shared" si="9"/>
         <v>46.073830714512354</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N21" s="10">
+        <f t="shared" si="10"/>
+        <v>1.9208300813616574</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>13</v>
       </c>
       <c r="B22">
-        <f>A22*25.4</f>
+        <f t="shared" si="0"/>
         <v>330.2</v>
       </c>
       <c r="C22">
         <v>57</v>
       </c>
       <c r="D22">
-        <f>_xlfn.CEILING.MATH(0.8*C22)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E22">
-        <f>C22*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F22">
-        <f>E22+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G22">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H22">
-        <f>G22*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I22">
-        <f>H22+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J22">
-        <f>(E22+H22)/2</f>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="K22" s="9">
-        <f>D22/G22</f>
+      <c r="K22" s="5">
+        <f t="shared" si="7"/>
         <v>2.4210526315789473</v>
       </c>
-      <c r="L22" s="9">
-        <f>B22/K22/PI()</f>
+      <c r="L22" s="5">
+        <f t="shared" si="8"/>
         <v>43.413316607388396</v>
       </c>
-      <c r="M22" s="9">
-        <f>L22 + 4*$C$6*_xlfn.CEILING.MATH(K22)</f>
+      <c r="M22" s="5">
+        <f t="shared" si="9"/>
         <v>49.413316607388396</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N22" s="10">
+        <f t="shared" si="10"/>
+        <v>1.7910151772076612</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>14</v>
       </c>
       <c r="B23">
-        <f>A23*25.4</f>
+        <f t="shared" si="0"/>
         <v>355.59999999999997</v>
       </c>
       <c r="C23">
         <v>57</v>
       </c>
       <c r="D23">
-        <f>_xlfn.CEILING.MATH(0.8*C23)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E23">
-        <f>C23*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F23">
-        <f>E23+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G23">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H23">
-        <f>G23*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I23">
-        <f>H23+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J23">
-        <f>(E23+H23)/2</f>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="K23" s="9">
-        <f>D23/G23</f>
+      <c r="K23" s="5">
+        <f t="shared" si="7"/>
         <v>2.4210526315789473</v>
       </c>
-      <c r="L23" s="9">
-        <f>B23/K23/PI()</f>
+      <c r="L23" s="5">
+        <f t="shared" si="8"/>
         <v>46.752802500264416</v>
       </c>
-      <c r="M23" s="9">
-        <f>L23 + 4*$C$6*_xlfn.CEILING.MATH(K23)</f>
+      <c r="M23" s="5">
+        <f t="shared" si="9"/>
         <v>52.752802500264416</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N23" s="10">
+        <f t="shared" si="10"/>
+        <v>1.6776359890937815</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>15</v>
       </c>
       <c r="B24">
-        <f>A24*25.4</f>
+        <f t="shared" si="0"/>
         <v>381</v>
       </c>
       <c r="C24">
         <v>57</v>
       </c>
       <c r="D24">
-        <f>_xlfn.CEILING.MATH(0.8*C24)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E24">
-        <f>C24*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F24">
-        <f>E24+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G24">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H24">
-        <f>G24*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I24">
-        <f>H24+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J24">
-        <f>(E24+H24)/2</f>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="K24" s="9">
-        <f>D24/G24</f>
+      <c r="K24" s="5">
+        <f t="shared" si="7"/>
         <v>2.4210526315789473</v>
       </c>
-      <c r="L24" s="9">
-        <f>B24/K24/PI()</f>
+      <c r="L24" s="5">
+        <f t="shared" si="8"/>
         <v>50.092288393140457</v>
       </c>
-      <c r="M24" s="9">
-        <f>L24 + 4*$C$6*_xlfn.CEILING.MATH(K24)</f>
+      <c r="M24" s="5">
+        <f t="shared" si="9"/>
         <v>56.092288393140457</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N24" s="10">
+        <f t="shared" si="10"/>
+        <v>1.5777569882640532</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>16</v>
       </c>
       <c r="B25">
-        <f>A25*25.4</f>
+        <f t="shared" si="0"/>
         <v>406.4</v>
       </c>
       <c r="C25">
         <v>57</v>
       </c>
       <c r="D25">
-        <f>_xlfn.CEILING.MATH(0.8*C25)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E25">
-        <f>C25*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F25">
-        <f>E25+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G25">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H25">
-        <f>G25*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I25">
-        <f>H25+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J25">
-        <f>(E25+H25)/2</f>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="K25" s="9">
-        <f>D25/G25</f>
+      <c r="K25" s="5">
+        <f t="shared" si="7"/>
         <v>2.4210526315789473</v>
       </c>
-      <c r="L25" s="9">
-        <f>B25/K25/PI()</f>
+      <c r="L25" s="5">
+        <f t="shared" si="8"/>
         <v>53.431774286016477</v>
       </c>
-      <c r="M25" s="9">
-        <f>L25 + 4*$C$6*_xlfn.CEILING.MATH(K25)</f>
+      <c r="M25" s="5">
+        <f t="shared" si="9"/>
         <v>59.431774286016477</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N25" s="10">
+        <f t="shared" si="10"/>
+        <v>1.4891024382696731</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>17</v>
       </c>
       <c r="B26">
-        <f>A26*25.4</f>
+        <f t="shared" si="0"/>
         <v>431.79999999999995</v>
       </c>
       <c r="C26">
         <v>57</v>
       </c>
       <c r="D26">
-        <f>_xlfn.CEILING.MATH(0.8*C26)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E26">
-        <f>C26*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F26">
-        <f>E26+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G26">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H26">
-        <f>G26*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I26">
-        <f>H26+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J26">
-        <f>(E26+H26)/2</f>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="K26" s="9">
-        <f>D26/G26</f>
+      <c r="K26" s="5">
+        <f t="shared" si="7"/>
         <v>2.4210526315789473</v>
       </c>
-      <c r="L26" s="9">
-        <f>B26/K26/PI()</f>
+      <c r="L26" s="5">
+        <f t="shared" si="8"/>
         <v>56.771260178892504</v>
       </c>
-      <c r="M26" s="9">
-        <f>L26 + 4*$C$6*_xlfn.CEILING.MATH(K26)</f>
+      <c r="M26" s="5">
+        <f t="shared" si="9"/>
         <v>62.771260178892504</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N26" s="10">
+        <f t="shared" si="10"/>
+        <v>1.4098808873325608</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>18</v>
       </c>
       <c r="B27">
-        <f>A27*25.4</f>
+        <f t="shared" si="0"/>
         <v>457.2</v>
       </c>
       <c r="C27">
         <v>57</v>
       </c>
       <c r="D27">
-        <f>_xlfn.CEILING.MATH(0.8*C27)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E27">
-        <f>C27*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F27">
-        <f>E27+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G27">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H27">
-        <f>G27*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I27">
-        <f>H27+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J27">
-        <f>(E27+H27)/2</f>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="K27" s="9">
-        <f>D27/G27</f>
+      <c r="K27" s="5">
+        <f t="shared" si="7"/>
         <v>2.4210526315789473</v>
       </c>
-      <c r="L27" s="9">
-        <f>B27/K27/PI()</f>
+      <c r="L27" s="5">
+        <f t="shared" si="8"/>
         <v>60.110746071768546</v>
       </c>
-      <c r="M27" s="9">
-        <f>L27 + 4*$C$6*_xlfn.CEILING.MATH(K27)</f>
+      <c r="M27" s="5">
+        <f t="shared" si="9"/>
         <v>66.110746071768546</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N27" s="10">
+        <f t="shared" si="10"/>
+        <v>1.338662853750374</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>19</v>
       </c>
       <c r="B28">
-        <f>A28*25.4</f>
+        <f t="shared" si="0"/>
         <v>482.59999999999997</v>
       </c>
       <c r="C28">
         <v>57</v>
       </c>
       <c r="D28">
-        <f>_xlfn.CEILING.MATH(0.8*C28)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E28">
-        <f>C28*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F28">
-        <f>E28+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G28">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H28">
-        <f>G28*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I28">
-        <f>H28+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J28">
-        <f>(E28+H28)/2</f>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="K28" s="9">
-        <f>D28/G28</f>
+      <c r="K28" s="5">
+        <f t="shared" si="7"/>
         <v>2.4210526315789473</v>
       </c>
-      <c r="L28" s="9">
-        <f>B28/K28/PI()</f>
+      <c r="L28" s="5">
+        <f t="shared" si="8"/>
         <v>63.450231964644566</v>
       </c>
-      <c r="M28" s="9">
-        <f>L28 + 4*$C$6*_xlfn.CEILING.MATH(K28)</f>
+      <c r="M28" s="5">
+        <f t="shared" si="9"/>
         <v>69.450231964644559</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N28" s="10">
+        <f t="shared" si="10"/>
+        <v>1.2742937999840407</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>20</v>
       </c>
       <c r="B29">
-        <f>A29*25.4</f>
+        <f t="shared" si="0"/>
         <v>508</v>
       </c>
       <c r="C29">
         <v>57</v>
       </c>
       <c r="D29">
-        <f>_xlfn.CEILING.MATH(0.8*C29)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E29">
-        <f>C29*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F29">
-        <f>E29+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G29">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H29">
-        <f>G29*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I29">
-        <f>H29+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J29">
-        <f>(E29+H29)/2</f>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="K29" s="9">
-        <f>D29/G29</f>
+      <c r="K29" s="5">
+        <f t="shared" si="7"/>
         <v>2.4210526315789473</v>
       </c>
-      <c r="L29" s="9">
-        <f>B29/K29/PI()</f>
+      <c r="L29" s="5">
+        <f t="shared" si="8"/>
         <v>66.7897178575206</v>
       </c>
-      <c r="M29" s="9">
-        <f>L29 + 4*$C$6*_xlfn.CEILING.MATH(K29)</f>
+      <c r="M29" s="5">
+        <f t="shared" si="9"/>
         <v>72.7897178575206</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N29" s="10">
+        <f t="shared" si="10"/>
+        <v>1.2158310624754842</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>21</v>
       </c>
       <c r="B30">
-        <f>A30*25.4</f>
+        <f t="shared" si="0"/>
         <v>533.4</v>
       </c>
       <c r="C30">
         <v>57</v>
       </c>
       <c r="D30">
-        <f>_xlfn.CEILING.MATH(0.8*C30)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E30">
-        <f>C30*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F30">
-        <f>E30+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G30">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H30">
-        <f>G30*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I30">
-        <f>H30+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J30">
-        <f>(E30+H30)/2</f>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="K30" s="9">
-        <f>D30/G30</f>
+      <c r="K30" s="5">
+        <f t="shared" si="7"/>
         <v>2.4210526315789473</v>
       </c>
-      <c r="L30" s="9">
-        <f>B30/K30/PI()</f>
+      <c r="L30" s="5">
+        <f t="shared" si="8"/>
         <v>70.129203750396627</v>
       </c>
-      <c r="M30" s="9">
-        <f>L30 + 4*$C$6*_xlfn.CEILING.MATH(K30)</f>
+      <c r="M30" s="5">
+        <f t="shared" si="9"/>
         <v>76.129203750396627</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N30" s="10">
+        <f t="shared" si="10"/>
+        <v>1.1624973812961878</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>22</v>
       </c>
       <c r="B31">
-        <f>A31*25.4</f>
+        <f t="shared" si="0"/>
         <v>558.79999999999995</v>
       </c>
       <c r="C31">
         <v>57</v>
       </c>
       <c r="D31">
-        <f>_xlfn.CEILING.MATH(0.8*C31)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E31">
-        <f>C31*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F31">
-        <f>E31+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G31">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H31">
-        <f>G31*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I31">
-        <f>H31+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J31">
-        <f>(E31+H31)/2</f>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="K31" s="9">
-        <f>D31/G31</f>
+      <c r="K31" s="5">
+        <f t="shared" si="7"/>
         <v>2.4210526315789473</v>
       </c>
-      <c r="L31" s="9">
-        <f>B31/K31/PI()</f>
+      <c r="L31" s="5">
+        <f t="shared" si="8"/>
         <v>73.468689643272654</v>
       </c>
-      <c r="M31" s="9">
-        <f>L31 + 4*$C$6*_xlfn.CEILING.MATH(K31)</f>
+      <c r="M31" s="5">
+        <f t="shared" si="9"/>
         <v>79.468689643272654</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N31" s="10">
+        <f t="shared" si="10"/>
+        <v>1.1136461466430116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>23</v>
       </c>
       <c r="B32">
-        <f>A32*25.4</f>
+        <f t="shared" si="0"/>
         <v>584.19999999999993</v>
       </c>
       <c r="C32">
         <v>57</v>
       </c>
       <c r="D32">
-        <f>_xlfn.CEILING.MATH(0.8*C32)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E32">
-        <f>C32*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F32">
-        <f>E32+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G32">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H32">
-        <f>G32*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I32">
-        <f>H32+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J32">
-        <f>(E32+H32)/2</f>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="K32" s="9">
-        <f>D32/G32</f>
+      <c r="K32" s="5">
+        <f t="shared" si="7"/>
         <v>2.4210526315789473</v>
       </c>
-      <c r="L32" s="9">
-        <f>B32/K32/PI()</f>
+      <c r="L32" s="5">
+        <f t="shared" si="8"/>
         <v>76.808175536148681</v>
       </c>
-      <c r="M32" s="9">
-        <f>L32 + 4*$C$6*_xlfn.CEILING.MATH(K32)</f>
+      <c r="M32" s="5">
+        <f t="shared" si="9"/>
         <v>82.808175536148681</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="N32" s="10">
+        <f t="shared" si="10"/>
+        <v>1.0687350545643484</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="1">
         <v>24</v>
       </c>
       <c r="B33" s="1">
-        <f>A33*25.4</f>
+        <f t="shared" si="0"/>
         <v>609.59999999999991</v>
       </c>
       <c r="C33" s="1">
         <v>57</v>
       </c>
       <c r="D33" s="1">
-        <f>_xlfn.CEILING.MATH(0.8*C33)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E33" s="1">
-        <f>C33*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F33" s="1">
-        <f>E33+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G33" s="1">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H33" s="1">
-        <f>G33*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I33" s="1">
-        <f>H33+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J33" s="1">
-        <f>(E33+H33)/2</f>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="K33" s="10">
-        <f>D33/G33</f>
+      <c r="K33" s="6">
+        <f t="shared" si="7"/>
         <v>2.4210526315789473</v>
       </c>
-      <c r="L33" s="10">
-        <f>B33/K33/PI()</f>
+      <c r="L33" s="6">
+        <f t="shared" si="8"/>
         <v>80.147661429024708</v>
       </c>
-      <c r="M33" s="10">
-        <f>L33 + 4*$C$6*_xlfn.CEILING.MATH(K33)</f>
+      <c r="M33" s="6">
+        <f t="shared" si="9"/>
         <v>86.147661429024708</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N33" s="10">
+        <f t="shared" si="10"/>
+        <v>1.0273058900491843</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>25</v>
       </c>
       <c r="B34">
-        <f>A34*25.4</f>
+        <f t="shared" si="0"/>
         <v>635</v>
       </c>
       <c r="C34">
         <v>57</v>
       </c>
       <c r="D34">
-        <f>_xlfn.CEILING.MATH(0.8*C34)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E34">
-        <f>C34*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F34">
-        <f>E34+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G34">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H34">
-        <f>G34*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I34">
-        <f>H34+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J34">
-        <f>(E34+H34)/2</f>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="K34" s="9">
-        <f>D34/G34</f>
+      <c r="K34" s="5">
+        <f t="shared" si="7"/>
         <v>2.4210526315789473</v>
       </c>
-      <c r="L34" s="9">
-        <f>B34/K34/PI()</f>
+      <c r="L34" s="5">
+        <f t="shared" si="8"/>
         <v>83.48714732190075</v>
       </c>
-      <c r="M34" s="9">
-        <f>L34 + 4*$C$6*_xlfn.CEILING.MATH(K34)</f>
+      <c r="M34" s="5">
+        <f t="shared" si="9"/>
         <v>89.48714732190075</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N34" s="10">
+        <f t="shared" si="10"/>
+        <v>0.98896883685039361</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>26</v>
       </c>
       <c r="B35">
-        <f>A35*25.4</f>
+        <f t="shared" si="0"/>
         <v>660.4</v>
       </c>
       <c r="C35">
         <v>57</v>
       </c>
       <c r="D35">
-        <f>_xlfn.CEILING.MATH(0.8*C35)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E35">
-        <f>C35*$C$1</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="F35">
-        <f>E35+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>88.5</v>
       </c>
       <c r="G35">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H35">
-        <f>G35*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I35">
-        <f>H35+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J35">
-        <f>(E35+H35)/2</f>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="K35" s="9">
-        <f>D35/G35</f>
+      <c r="K35" s="5">
+        <f t="shared" si="7"/>
         <v>2.4210526315789473</v>
       </c>
-      <c r="L35" s="9">
-        <f>B35/K35/PI()</f>
+      <c r="L35" s="5">
+        <f t="shared" si="8"/>
         <v>86.826633214776791</v>
       </c>
-      <c r="M35" s="9">
-        <f>L35 + 4*$C$6*_xlfn.CEILING.MATH(K35)</f>
+      <c r="M35" s="5">
+        <f t="shared" si="9"/>
         <v>92.826633214776791</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N35" s="10">
+        <f t="shared" si="10"/>
+        <v>0.95339017408111659</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>27</v>
       </c>
       <c r="B36">
-        <f>A36*25.4</f>
+        <f t="shared" si="0"/>
         <v>685.8</v>
       </c>
       <c r="C36">
         <v>58</v>
       </c>
       <c r="D36">
-        <f>_xlfn.CEILING.MATH(0.8*C36)</f>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="E36">
-        <f>C36*$C$1</f>
+        <f t="shared" si="2"/>
         <v>87</v>
       </c>
       <c r="F36">
-        <f>E36+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>90</v>
       </c>
       <c r="G36">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H36">
-        <f>G36*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I36">
-        <f>H36+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J36">
-        <f>(E36+H36)/2</f>
+        <f t="shared" si="6"/>
         <v>57.75</v>
       </c>
-      <c r="K36" s="9">
-        <f>D36/G36</f>
+      <c r="K36" s="5">
+        <f t="shared" si="7"/>
         <v>2.4736842105263159</v>
       </c>
-      <c r="L36" s="9">
-        <f>B36/K36/PI()</f>
+      <c r="L36" s="5">
+        <f t="shared" si="8"/>
         <v>88.247691041532534</v>
       </c>
-      <c r="M36" s="9">
-        <f>L36 + 4*$C$6*_xlfn.CEILING.MATH(K36)</f>
+      <c r="M36" s="5">
+        <f t="shared" si="9"/>
         <v>94.247691041532534</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N36" s="10">
+        <f t="shared" si="10"/>
+        <v>0.95493055591504428</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>28</v>
       </c>
       <c r="B37">
-        <f>A37*25.4</f>
+        <f t="shared" si="0"/>
         <v>711.19999999999993</v>
       </c>
       <c r="C37">
         <v>59</v>
       </c>
       <c r="D37">
-        <f>_xlfn.CEILING.MATH(0.8*C37)</f>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="E37">
-        <f>C37*$C$1</f>
+        <f t="shared" si="2"/>
         <v>88.5</v>
       </c>
       <c r="F37">
-        <f>E37+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>91.5</v>
       </c>
       <c r="G37">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H37">
-        <f>G37*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I37">
-        <f>H37+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J37">
-        <f>(E37+H37)/2</f>
+        <f t="shared" si="6"/>
         <v>58.5</v>
       </c>
-      <c r="K37" s="9">
-        <f>D37/G37</f>
+      <c r="K37" s="5">
+        <f t="shared" si="7"/>
         <v>2.5263157894736841</v>
       </c>
-      <c r="L37" s="9">
-        <f>B37/K37/PI()</f>
+      <c r="L37" s="5">
+        <f t="shared" si="8"/>
         <v>89.609538125506802</v>
       </c>
-      <c r="M37" s="9">
-        <f>L37 + 4*$C$6*_xlfn.CEILING.MATH(K37)</f>
+      <c r="M37" s="5">
+        <f t="shared" si="9"/>
         <v>95.609538125506802</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N37" s="10">
+        <f t="shared" si="10"/>
+        <v>0.95701748794024921</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>29</v>
       </c>
       <c r="B38">
-        <f>A38*25.4</f>
+        <f t="shared" si="0"/>
         <v>736.59999999999991</v>
       </c>
       <c r="C38">
         <v>61</v>
       </c>
       <c r="D38">
-        <f>_xlfn.CEILING.MATH(0.8*C38)</f>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="E38">
-        <f>C38*$C$1</f>
+        <f t="shared" si="2"/>
         <v>91.5</v>
       </c>
       <c r="F38">
-        <f>E38+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>94.5</v>
       </c>
       <c r="G38">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H38">
-        <f>G38*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I38">
-        <f>H38+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J38">
-        <f>(E38+H38)/2</f>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
-      <c r="K38" s="9">
-        <f>D38/G38</f>
+      <c r="K38" s="5">
+        <f t="shared" si="7"/>
         <v>2.5789473684210527</v>
       </c>
-      <c r="L38" s="9">
-        <f>B38/K38/PI()</f>
+      <c r="L38" s="5">
+        <f t="shared" si="8"/>
         <v>90.915799614216809</v>
       </c>
-      <c r="M38" s="9">
-        <f>L38 + 4*$C$6*_xlfn.CEILING.MATH(K38)</f>
+      <c r="M38" s="5">
+        <f t="shared" si="9"/>
         <v>96.915799614216809</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N38" s="10">
+        <f t="shared" si="10"/>
+        <v>0.9750732117587313</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>30</v>
       </c>
       <c r="B39">
-        <f>A39*25.4</f>
+        <f t="shared" si="0"/>
         <v>762</v>
       </c>
       <c r="C39">
         <v>62</v>
       </c>
       <c r="D39">
-        <f>_xlfn.CEILING.MATH(0.8*C39)</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="E39">
-        <f>C39*$C$1</f>
+        <f t="shared" si="2"/>
         <v>93</v>
       </c>
       <c r="F39">
-        <f>E39+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>96</v>
       </c>
       <c r="G39">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H39">
-        <f>G39*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I39">
-        <f>H39+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J39">
-        <f>(E39+H39)/2</f>
+        <f t="shared" si="6"/>
         <v>60.75</v>
       </c>
-      <c r="K39" s="9">
-        <f>D39/G39</f>
+      <c r="K39" s="5">
+        <f t="shared" si="7"/>
         <v>2.6315789473684212</v>
       </c>
-      <c r="L39" s="9">
-        <f>B39/K39/PI()</f>
+      <c r="L39" s="5">
+        <f t="shared" si="8"/>
         <v>92.169810643378426</v>
       </c>
-      <c r="M39" s="9">
-        <f>L39 + 4*$C$6*_xlfn.CEILING.MATH(K39)</f>
+      <c r="M39" s="5">
+        <f t="shared" si="9"/>
         <v>98.169810643378426</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N39" s="10">
+        <f t="shared" si="10"/>
+        <v>0.97789737365124707</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>31</v>
       </c>
       <c r="B40">
-        <f>A40*25.4</f>
+        <f t="shared" si="0"/>
         <v>787.4</v>
       </c>
       <c r="C40">
         <v>62</v>
       </c>
       <c r="D40">
-        <f>_xlfn.CEILING.MATH(0.8*C40)</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="E40">
-        <f>C40*$C$1</f>
+        <f t="shared" si="2"/>
         <v>93</v>
       </c>
       <c r="F40">
-        <f>E40+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>96</v>
       </c>
       <c r="G40">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H40">
-        <f>G40*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I40">
-        <f>H40+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J40">
-        <f>(E40+H40)/2</f>
+        <f t="shared" si="6"/>
         <v>60.75</v>
       </c>
-      <c r="K40" s="9">
-        <f>D40/G40</f>
+      <c r="K40" s="5">
+        <f t="shared" si="7"/>
         <v>2.6315789473684212</v>
       </c>
-      <c r="L40" s="9">
-        <f>B40/K40/PI()</f>
+      <c r="L40" s="5">
+        <f t="shared" si="8"/>
         <v>95.242137664824369</v>
       </c>
-      <c r="M40" s="9">
-        <f>L40 + 4*$C$6*_xlfn.CEILING.MATH(K40)</f>
+      <c r="M40" s="5">
+        <f t="shared" si="9"/>
         <v>101.24213766482437</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N40" s="10">
+        <f t="shared" si="10"/>
+        <v>0.94822178012302383</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>32</v>
       </c>
       <c r="B41">
-        <f>A41*25.4</f>
+        <f t="shared" si="0"/>
         <v>812.8</v>
       </c>
       <c r="C41">
         <v>63</v>
       </c>
       <c r="D41">
-        <f>_xlfn.CEILING.MATH(0.8*C41)</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="E41">
-        <f>C41*$C$1</f>
+        <f t="shared" si="2"/>
         <v>94.5</v>
       </c>
       <c r="F41">
-        <f>E41+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>97.5</v>
       </c>
       <c r="G41">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H41">
-        <f>G41*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I41">
-        <f>H41+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J41">
-        <f>(E41+H41)/2</f>
+        <f t="shared" si="6"/>
         <v>61.5</v>
       </c>
-      <c r="K41" s="9">
-        <f>D41/G41</f>
+      <c r="K41" s="5">
+        <f t="shared" si="7"/>
         <v>2.6842105263157894</v>
       </c>
-      <c r="L41" s="9">
-        <f>B41/K41/PI()</f>
+      <c r="L41" s="5">
+        <f t="shared" si="8"/>
         <v>96.386730084578758</v>
       </c>
-      <c r="M41" s="9">
-        <f>L41 + 4*$C$6*_xlfn.CEILING.MATH(K41)</f>
+      <c r="M41" s="5">
+        <f t="shared" si="9"/>
         <v>102.38673008457876</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N41" s="10">
+        <f t="shared" si="10"/>
+        <v>0.95227184147260124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>33</v>
       </c>
       <c r="B42">
-        <f>A42*25.4</f>
+        <f t="shared" si="0"/>
         <v>838.19999999999993</v>
       </c>
       <c r="C42">
         <v>64</v>
       </c>
       <c r="D42">
-        <f>_xlfn.CEILING.MATH(0.8*C42)</f>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="E42">
-        <f>C42*$C$1</f>
+        <f t="shared" si="2"/>
         <v>96</v>
       </c>
       <c r="F42">
-        <f>E42+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>99</v>
       </c>
       <c r="G42">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H42">
-        <f>G42*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I42">
-        <f>H42+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J42">
-        <f>(E42+H42)/2</f>
+        <f t="shared" si="6"/>
         <v>62.25</v>
       </c>
-      <c r="K42" s="9">
-        <f>D42/G42</f>
+      <c r="K42" s="5">
+        <f t="shared" si="7"/>
         <v>2.736842105263158</v>
       </c>
-      <c r="L42" s="9">
-        <f>B42/K42/PI()</f>
+      <c r="L42" s="5">
+        <f t="shared" si="8"/>
         <v>97.487299718957942</v>
       </c>
-      <c r="M42" s="9">
-        <f>L42 + 4*$C$6*_xlfn.CEILING.MATH(K42)</f>
+      <c r="M42" s="5">
+        <f t="shared" si="9"/>
         <v>103.48729971895794</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N42" s="10">
+        <f t="shared" si="10"/>
+        <v>0.9566391264324785</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>34</v>
       </c>
       <c r="B43">
-        <f>A43*25.4</f>
+        <f t="shared" si="0"/>
         <v>863.59999999999991</v>
       </c>
       <c r="C43">
         <v>66</v>
       </c>
       <c r="D43">
-        <f>_xlfn.CEILING.MATH(0.8*C43)</f>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="E43">
-        <f>C43*$C$1</f>
+        <f t="shared" si="2"/>
         <v>99</v>
       </c>
       <c r="F43">
-        <f>E43+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>102</v>
       </c>
       <c r="G43">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H43">
-        <f>G43*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I43">
-        <f>H43+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J43">
-        <f>(E43+H43)/2</f>
+        <f t="shared" si="6"/>
         <v>63.75</v>
       </c>
-      <c r="K43" s="9">
-        <f>D43/G43</f>
+      <c r="K43" s="5">
+        <f t="shared" si="7"/>
         <v>2.7894736842105261</v>
       </c>
-      <c r="L43" s="9">
-        <f>B43/K43/PI()</f>
+      <c r="L43" s="5">
+        <f t="shared" si="8"/>
         <v>98.54633842373795</v>
       </c>
-      <c r="M43" s="9">
-        <f>L43 + 4*$C$6*_xlfn.CEILING.MATH(K43)</f>
+      <c r="M43" s="5">
+        <f t="shared" si="9"/>
         <v>104.54633842373795</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N43" s="10">
+        <f t="shared" si="10"/>
+        <v>0.97564392534325439</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>35</v>
       </c>
       <c r="B44">
-        <f>A44*25.4</f>
+        <f t="shared" si="0"/>
         <v>889</v>
       </c>
       <c r="C44">
         <v>66</v>
       </c>
       <c r="D44">
-        <f>_xlfn.CEILING.MATH(0.8*C44)</f>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="E44">
-        <f>C44*$C$1</f>
+        <f t="shared" si="2"/>
         <v>99</v>
       </c>
       <c r="F44">
-        <f>E44+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>102</v>
       </c>
       <c r="G44">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H44">
-        <f>G44*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I44">
-        <f>H44+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J44">
-        <f>(E44+H44)/2</f>
+        <f t="shared" si="6"/>
         <v>63.75</v>
       </c>
-      <c r="K44" s="9">
-        <f>D44/G44</f>
+      <c r="K44" s="5">
+        <f t="shared" si="7"/>
         <v>2.7894736842105261</v>
       </c>
-      <c r="L44" s="9">
-        <f>B44/K44/PI()</f>
+      <c r="L44" s="5">
+        <f t="shared" si="8"/>
         <v>101.44476014208318</v>
       </c>
-      <c r="M44" s="9">
-        <f>L44 + 4*$C$6*_xlfn.CEILING.MATH(K44)</f>
+      <c r="M44" s="5">
+        <f t="shared" si="9"/>
         <v>107.44476014208318</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N44" s="10">
+        <f t="shared" si="10"/>
+        <v>0.94932502864836665</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>36</v>
       </c>
       <c r="B45">
-        <f>A45*25.4</f>
+        <f t="shared" si="0"/>
         <v>914.4</v>
       </c>
       <c r="C45">
         <v>67</v>
       </c>
       <c r="D45">
-        <f>_xlfn.CEILING.MATH(0.8*C45)</f>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="E45">
-        <f>C45*$C$1</f>
+        <f t="shared" si="2"/>
         <v>100.5</v>
       </c>
       <c r="F45">
-        <f>E45+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>103.5</v>
       </c>
       <c r="G45">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H45">
-        <f>G45*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I45">
-        <f>H45+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J45">
-        <f>(E45+H45)/2</f>
+        <f t="shared" si="6"/>
         <v>64.5</v>
       </c>
-      <c r="K45" s="9">
-        <f>D45/G45</f>
+      <c r="K45" s="5">
+        <f t="shared" si="7"/>
         <v>2.8421052631578947</v>
       </c>
-      <c r="L45" s="9">
-        <f>B45/K45/PI()</f>
+      <c r="L45" s="5">
+        <f t="shared" si="8"/>
         <v>102.41090071486492</v>
       </c>
-      <c r="M45" s="9">
-        <f>L45 + 4*$C$6*_xlfn.CEILING.MATH(K45)</f>
+      <c r="M45" s="5">
+        <f t="shared" si="9"/>
         <v>108.41090071486492</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N45" s="10">
+        <f t="shared" si="10"/>
+        <v>0.95470104313789217</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>37</v>
       </c>
       <c r="B46">
-        <f>A46*25.4</f>
+        <f t="shared" si="0"/>
         <v>939.8</v>
       </c>
       <c r="C46">
         <v>68</v>
       </c>
       <c r="D46">
-        <f>_xlfn.CEILING.MATH(0.8*C46)</f>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="E46">
-        <f>C46*$C$1</f>
+        <f t="shared" si="2"/>
         <v>102</v>
       </c>
       <c r="F46">
-        <f>E46+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>105</v>
       </c>
       <c r="G46">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H46">
-        <f>G46*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I46">
-        <f>H46+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J46">
-        <f>(E46+H46)/2</f>
+        <f t="shared" si="6"/>
         <v>65.25</v>
       </c>
-      <c r="K46" s="9">
-        <f>D46/G46</f>
+      <c r="K46" s="5">
+        <f t="shared" si="7"/>
         <v>2.8947368421052633</v>
       </c>
-      <c r="L46" s="9">
-        <f>B46/K46/PI()</f>
+      <c r="L46" s="5">
+        <f t="shared" si="8"/>
         <v>103.34190890318186</v>
       </c>
-      <c r="M46" s="9">
-        <f>L46 + 4*$C$6*_xlfn.CEILING.MATH(K46)</f>
+      <c r="M46" s="5">
+        <f t="shared" si="9"/>
         <v>109.34190890318186</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N46" s="10">
+        <f t="shared" si="10"/>
+        <v>0.96029053318406521</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>38</v>
       </c>
       <c r="B47">
-        <f>A47*25.4</f>
+        <f t="shared" si="0"/>
         <v>965.19999999999993</v>
       </c>
       <c r="C47">
         <v>69</v>
       </c>
       <c r="D47">
-        <f>_xlfn.CEILING.MATH(0.8*C47)</f>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="E47">
-        <f>C47*$C$1</f>
+        <f t="shared" si="2"/>
         <v>103.5</v>
       </c>
       <c r="F47">
-        <f>E47+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>106.5</v>
       </c>
       <c r="G47">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H47">
-        <f>G47*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I47">
-        <f>H47+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J47">
-        <f>(E47+H47)/2</f>
+        <f t="shared" si="6"/>
         <v>66</v>
       </c>
-      <c r="K47" s="9">
-        <f>D47/G47</f>
+      <c r="K47" s="5">
+        <f t="shared" si="7"/>
         <v>2.9473684210526314</v>
       </c>
-      <c r="L47" s="9">
-        <f>B47/K47/PI()</f>
+      <c r="L47" s="5">
+        <f t="shared" si="8"/>
         <v>104.23966679905892</v>
       </c>
-      <c r="M47" s="9">
-        <f>L47 + 4*$C$6*_xlfn.CEILING.MATH(K47)</f>
+      <c r="M47" s="5">
+        <f t="shared" si="9"/>
         <v>110.23966679905892</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N47" s="10">
+        <f t="shared" si="10"/>
+        <v>0.96607694029159707</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>39</v>
       </c>
       <c r="B48">
-        <f>A48*25.4</f>
+        <f t="shared" si="0"/>
         <v>990.59999999999991</v>
       </c>
       <c r="C48">
         <v>70</v>
       </c>
       <c r="D48">
-        <f>_xlfn.CEILING.MATH(0.8*C48)</f>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="E48">
-        <f>C48*$C$1</f>
+        <f t="shared" si="2"/>
         <v>105</v>
       </c>
       <c r="F48">
-        <f>E48+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>108</v>
       </c>
       <c r="G48">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H48">
-        <f>G48*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I48">
-        <f>H48+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J48">
-        <f>(E48+H48)/2</f>
+        <f t="shared" si="6"/>
         <v>66.75</v>
       </c>
-      <c r="K48" s="9">
-        <f>D48/G48</f>
+      <c r="K48" s="5">
+        <f t="shared" si="7"/>
         <v>2.9473684210526314</v>
       </c>
-      <c r="L48" s="9">
-        <f>B48/K48/PI()</f>
+      <c r="L48" s="5">
+        <f t="shared" si="8"/>
         <v>106.98281592534995</v>
       </c>
-      <c r="M48" s="9">
-        <f>L48 + 4*$C$6*_xlfn.CEILING.MATH(K48)</f>
+      <c r="M48" s="5">
+        <f t="shared" si="9"/>
         <v>112.98281592534995</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N48" s="10">
+        <f t="shared" si="10"/>
+        <v>0.95589757712675349</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>40</v>
       </c>
       <c r="B49">
-        <f>A49*25.4</f>
+        <f t="shared" si="0"/>
         <v>1016</v>
       </c>
       <c r="C49">
         <v>71</v>
       </c>
       <c r="D49">
-        <f>_xlfn.CEILING.MATH(0.8*C49)</f>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="E49">
-        <f>C49*$C$1</f>
+        <f t="shared" si="2"/>
         <v>106.5</v>
       </c>
       <c r="F49">
-        <f>E49+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>109.5</v>
       </c>
       <c r="G49">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H49">
-        <f>G49*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I49">
-        <f>H49+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J49">
-        <f>(E49+H49)/2</f>
+        <f t="shared" si="6"/>
         <v>67.5</v>
       </c>
-      <c r="K49" s="9">
-        <f>D49/G49</f>
+      <c r="K49" s="5">
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="L49" s="9">
-        <f>B49/K49/PI()</f>
+      <c r="L49" s="5">
+        <f t="shared" si="8"/>
         <v>107.80094812091045</v>
       </c>
-      <c r="M49" s="9">
-        <f>L49 + 4*$C$6*_xlfn.CEILING.MATH(K49)</f>
+      <c r="M49" s="5">
+        <f t="shared" si="9"/>
         <v>113.80094812091045</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N49" s="10">
+        <f t="shared" si="10"/>
+        <v>0.96220639465726765</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>41</v>
       </c>
       <c r="B50">
-        <f>A50*25.4</f>
+        <f t="shared" si="0"/>
         <v>1041.3999999999999</v>
       </c>
       <c r="C50">
         <v>73</v>
       </c>
       <c r="D50">
-        <f>_xlfn.CEILING.MATH(0.8*C50)</f>
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="E50">
-        <f>C50*$C$1</f>
+        <f t="shared" si="2"/>
         <v>109.5</v>
       </c>
       <c r="F50">
-        <f>E50+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>112.5</v>
       </c>
       <c r="G50">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H50">
-        <f>G50*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I50">
-        <f>H50+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J50">
-        <f>(E50+H50)/2</f>
+        <f t="shared" si="6"/>
         <v>69</v>
       </c>
-      <c r="K50" s="9">
-        <f>D50/G50</f>
+      <c r="K50" s="5">
+        <f t="shared" si="7"/>
         <v>3.1052631578947367</v>
       </c>
-      <c r="L50" s="9">
-        <f>B50/K50/PI()</f>
+      <c r="L50" s="5">
+        <f t="shared" si="8"/>
         <v>106.75034566041005</v>
       </c>
-      <c r="M50" s="9">
-        <f>L50 + 4*$C$6*_xlfn.CEILING.MATH(K50)</f>
+      <c r="M50" s="5">
+        <f t="shared" si="9"/>
         <v>114.75034566041005</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="N50" s="10">
+        <f t="shared" si="10"/>
+        <v>0.98038920364501836</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>42</v>
       </c>
       <c r="B51">
-        <f>A51*25.4</f>
+        <f t="shared" si="0"/>
         <v>1066.8</v>
       </c>
       <c r="C51">
         <v>73</v>
       </c>
       <c r="D51">
-        <f>_xlfn.CEILING.MATH(0.8*C51)</f>
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="E51">
-        <f>C51*$C$1</f>
+        <f t="shared" si="2"/>
         <v>109.5</v>
       </c>
       <c r="F51">
-        <f>E51+2*$C$1</f>
+        <f t="shared" si="3"/>
         <v>112.5</v>
       </c>
       <c r="G51">
-        <f>_xlfn.CEILING.MATH(($C$4 + 2*(1+$C$2)*$C$1) / $C$1)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H51">
-        <f>G51*$C$1</f>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="I51">
-        <f>H51+2*$C$1</f>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J51">
-        <f>(E51+H51)/2</f>
+        <f t="shared" si="6"/>
         <v>69</v>
       </c>
-      <c r="K51" s="9">
-        <f>D51/G51</f>
+      <c r="K51" s="5">
+        <f t="shared" si="7"/>
         <v>3.1052631578947367</v>
       </c>
-      <c r="L51" s="9">
-        <f>B51/K51/PI()</f>
+      <c r="L51" s="5">
+        <f t="shared" si="8"/>
         <v>109.35401262773713</v>
       </c>
-      <c r="M51" s="9">
-        <f>L51 + 4*$C$6*_xlfn.CEILING.MATH(K51)</f>
+      <c r="M51" s="5">
+        <f t="shared" si="9"/>
         <v>117.35401262773713</v>
+      </c>
+      <c r="N51" s="10">
+        <f t="shared" si="10"/>
+        <v>0.95863786402315254</v>
       </c>
     </row>
   </sheetData>
@@ -2872,9 +4494,9 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="L8:M8"/>
   </mergeCells>
-  <conditionalFormatting sqref="M10:M51">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
-      <formula>2*J10 - $C$5</formula>
+  <conditionalFormatting sqref="I10:I51">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>M10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:L51">
@@ -2882,11 +4504,26 @@
       <formula>$C$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10:I51">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
-      <formula>M10</formula>
+  <conditionalFormatting sqref="M10:M51">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+      <formula>2*J10 - $C$5</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D4FD04-CC5E-4C3D-8AEB-E4702795F5BB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>